<commit_message>
added the GraphRunner so it will run independently the simulations
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -65,48 +65,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.005483999491233108</v>
+        <v>0.005857887150227237</v>
       </c>
       <c r="B1" t="n">
-        <v>0.004242663123729053</v>
+        <v>0.005033460283055886</v>
       </c>
       <c r="C1" t="n">
-        <v>0.0019590921065850697</v>
+        <v>0.005339797749090689</v>
       </c>
       <c r="D1" t="n">
-        <v>2.2388734496209503E-4</v>
+        <v>0.0053896520392816985</v>
       </c>
       <c r="E1" t="n">
-        <v>0.0060547770132278545</v>
+        <v>2.358906964794187E-4</v>
       </c>
       <c r="F1" t="n">
-        <v>1.3456487048702766E308</v>
+        <v>3.1679263854308676E307</v>
       </c>
       <c r="G1" t="n">
-        <v>1.3421602543584315E307</v>
+        <v>1.3589459247596537E308</v>
       </c>
       <c r="H1" t="n">
-        <v>6.237707630957962E307</v>
+        <v>7.482971686277037E307</v>
       </c>
       <c r="I1" t="n">
-        <v>6.53399316510401E307</v>
+        <v>1.2483570308335637E308</v>
       </c>
       <c r="J1" t="n">
-        <v>9.014452659765037E307</v>
+        <v>1.5131464316013779E308</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.0</v>
+        <v>27.0</v>
       </c>
       <c r="B2" t="n">
-        <v>136.0</v>
+        <v>0.0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="E2" t="n">
         <v>0.0</v>
@@ -142,34 +142,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.006563889275809197</v>
+        <v>2.8560776309376505E-4</v>
       </c>
       <c r="B1" t="n">
-        <v>0.005467310998422768</v>
+        <v>0.00372002482552455</v>
       </c>
       <c r="C1" t="n">
-        <v>0.005050280087365146</v>
+        <v>0.006483710142371962</v>
       </c>
       <c r="D1" t="n">
-        <v>0.006866105379382536</v>
+        <v>0.003743810130259544</v>
       </c>
       <c r="E1" t="n">
-        <v>0.005948914991065626</v>
+        <v>0.004176234691075986</v>
       </c>
       <c r="F1" t="n">
-        <v>1.1392928267119121E306</v>
+        <v>1.2209648322088105E308</v>
       </c>
       <c r="G1" t="n">
-        <v>4.887248683865666E307</v>
+        <v>1.3661546677709258E307</v>
       </c>
       <c r="H1" t="n">
-        <v>3.554824219578909E307</v>
+        <v>3.461662078480697E307</v>
       </c>
       <c r="I1" t="n">
-        <v>1.6841559112297773E308</v>
+        <v>1.6768333882002263E308</v>
       </c>
       <c r="J1" t="n">
-        <v>3.657209378327557E307</v>
+        <v>1.9304363359560103E307</v>
       </c>
     </row>
     <row r="2">
@@ -180,13 +180,13 @@
         <v>500.0</v>
       </c>
       <c r="C2" t="n">
-        <v>500.0</v>
+        <v>394.0</v>
       </c>
       <c r="D2" t="n">
         <v>500.0</v>
       </c>
       <c r="E2" t="n">
-        <v>396.0</v>
+        <v>500.0</v>
       </c>
       <c r="F2" t="n">
         <v>0.0</v>
@@ -219,66 +219,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.10284799267662749</v>
+        <v>0.01553666732814921</v>
       </c>
       <c r="B1" t="n">
-        <v>0.07388355041705583</v>
+        <v>0.04467448688954686</v>
       </c>
       <c r="C1" t="n">
-        <v>0.10719556621803945</v>
+        <v>0.07668788255007811</v>
       </c>
       <c r="D1" t="n">
-        <v>0.06427641316294809</v>
+        <v>0.10937757571686146</v>
       </c>
       <c r="E1" t="n">
-        <v>0.10829482754075677</v>
+        <v>0.054827703426204036</v>
       </c>
       <c r="F1" t="n">
-        <v>1.375624347927052E308</v>
+        <v>9.671823698659732E307</v>
       </c>
       <c r="G1" t="n">
-        <v>2.0967508523338298E307</v>
+        <v>9.941426995253211E306</v>
       </c>
       <c r="H1" t="n">
-        <v>4.540783929668453E307</v>
+        <v>1.6920586194097304E308</v>
       </c>
       <c r="I1" t="n">
-        <v>1.507895134198964E307</v>
+        <v>1.5914341940751387E308</v>
       </c>
       <c r="J1" t="n">
-        <v>1.3460295018345307E308</v>
+        <v>8.300351259686377E307</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="C2" t="n">
-        <v>93.0</v>
+        <v>14.0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="E2" t="n">
-        <v>462.0</v>
+        <v>15.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>